<commit_message>
Thêm vấn đề và giải pháp về quy định
</commit_message>
<xml_diff>
--- a/03. Hinh anh - Noi dung/02. Facebook/01. San Pham/TongHopSanPham.xlsx
+++ b/03. Hinh anh - Noi dung/02. Facebook/01. San Pham/TongHopSanPham.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="38">
   <si>
     <t>STT</t>
   </si>
@@ -126,13 +126,25 @@
   </si>
   <si>
     <t>AoDaiBeTrai\AoDaiBeTraiTrangDo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">330k </t>
+  </si>
+  <si>
+    <t>Bộ đồ vest màu xanh</t>
+  </si>
+  <si>
+    <t>Áo vest màu xanh, không gồm áo trong</t>
+  </si>
+  <si>
+    <t>AoDaiBeTrai\BoDoVestBeTrai\79145105_565024997663091_6173803411104858112_n.jpg</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -161,6 +173,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF444950"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -183,13 +201,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="16" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -471,10 +491,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H6"/>
+  <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -629,6 +649,9 @@
       <c r="D6" s="1" t="s">
         <v>29</v>
       </c>
+      <c r="E6" s="4" t="s">
+        <v>34</v>
+      </c>
       <c r="F6" s="1" t="s">
         <v>30</v>
       </c>
@@ -637,6 +660,32 @@
       </c>
       <c r="H6" s="1" t="s">
         <v>18</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
+        <v>6</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C7" s="5">
+        <v>43787</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E7" s="1">
+        <v>340</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>21</v>
       </c>
     </row>
   </sheetData>
@@ -646,8 +695,9 @@
     <hyperlink ref="G5" r:id="rId3"/>
     <hyperlink ref="G6" r:id="rId4"/>
     <hyperlink ref="G3" r:id="rId5"/>
+    <hyperlink ref="G7" r:id="rId6"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId6"/>
+  <pageSetup orientation="portrait" r:id="rId7"/>
 </worksheet>
 </file>
</xml_diff>